<commit_message>
Added model history and details files
</commit_message>
<xml_diff>
--- a/Segment2/ML_Models_Chronological.xlsx
+++ b/Segment2/ML_Models_Chronological.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuti\Desktop\Class Folder\MODULE20_FinalProject\UCB_COVID_Prediction_Model\UCB_COVID_Prediction_Model\Segment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583DAAFB-F662-41B0-8DCC-B69788C8F649}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FD4EE8-47B7-4B5D-8DC9-F5D056E3DCE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23865" yWindow="-150" windowWidth="20460" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26820" yWindow="-210" windowWidth="20460" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Models" sheetId="1" r:id="rId1"/>
+    <sheet name="ML_Models_Performance" sheetId="1" r:id="rId1"/>
     <sheet name="Model Owners" sheetId="3" r:id="rId2"/>
-    <sheet name="Epochs" sheetId="2" r:id="rId3"/>
+    <sheet name="Performance@30-50Epochs" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="54">
   <si>
     <t>Loss</t>
   </si>
@@ -289,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,6 +318,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -603,7 +615,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E2" sqref="E2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -612,7 +624,7 @@
     <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" style="1" customWidth="1"/>
@@ -649,7 +661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -674,7 +686,7 @@
       <c r="H2" s="3">
         <v>0.66149999999999998</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -750,16 +762,16 @@
         <v>16</v>
       </c>
       <c r="E5" s="5">
-        <v>0.6492</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="F5" s="3">
-        <v>0.90149999999999997</v>
+        <v>0.92779999999999996</v>
       </c>
       <c r="G5" s="3">
-        <v>0.65559999999999996</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="H5" s="3">
-        <v>0.89580000000000004</v>
+        <v>0.83679999999999999</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>28</v>
@@ -808,16 +820,16 @@
         <v>18</v>
       </c>
       <c r="E7" s="5">
-        <v>0.2676</v>
+        <v>0.1792</v>
       </c>
       <c r="F7" s="3">
-        <v>0.90629999999999999</v>
+        <v>0.93820000000000003</v>
       </c>
       <c r="G7" s="5">
-        <v>0.41239999999999999</v>
+        <v>0.36359999999999998</v>
       </c>
       <c r="H7" s="5">
-        <v>0.83360000000000001</v>
+        <v>0.86629999999999996</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>26</v>
@@ -837,16 +849,16 @@
         <v>19</v>
       </c>
       <c r="E8" s="3">
-        <v>0.58919999999999995</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="F8" s="3">
-        <v>0.96540000000000004</v>
+        <v>0.96940000000000004</v>
       </c>
       <c r="G8" s="3">
-        <v>0.68610000000000004</v>
+        <v>0.35070000000000001</v>
       </c>
       <c r="H8" s="3">
-        <v>0.8619</v>
+        <v>0.87160000000000004</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>28</v>
@@ -889,19 +901,23 @@
         <v>24</v>
       </c>
       <c r="C10" s="3">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="5">
-        <v>1.1971000000000001</v>
+        <v>0.36030000000000001</v>
       </c>
       <c r="F10" s="5">
-        <v>0.3543</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+        <v>0.86529999999999996</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.30609999999999998</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.87480000000000002</v>
+      </c>
       <c r="I10" s="12" t="s">
         <v>28</v>
       </c>
@@ -990,402 +1006,449 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCE48E4-EBFB-4242-A074-DA02F0FA4228}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="38" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="38" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.5703125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="E2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="F2" s="7">
         <v>30</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5">
+      <c r="H2" s="5">
         <v>0.19089999999999999</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>0.93600000000000005</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>1.6881999999999999</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>0.66149999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="E3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <v>30</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="5">
         <v>0.13539999999999999</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>0.95479999999999998</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3" s="5">
         <v>2.6053000000000002</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="5">
         <v>0.61809999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="E4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>30</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <v>0.24229999999999999</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>0.91720000000000002</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="5">
         <v>0.95509999999999995</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>0.68920000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="E5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>50</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="5">
         <v>0.6492</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>0.90149999999999997</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>0.65559999999999996</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>0.89580000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="E6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>100</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <v>0.1842</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>0.93669999999999998</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>0.39489999999999997</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="E7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>50</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="5">
         <v>0.2676</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>0.90629999999999999</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J7" s="5">
         <v>0.41239999999999999</v>
       </c>
-      <c r="J7" s="5">
+      <c r="K7" s="5">
         <v>0.83360000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="E8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>50</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>0.58919999999999995</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>0.96540000000000004</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>0.68610000000000004</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>0.8619</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3">
+        <v>50</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.3987</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.85540000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3">
         <v>23</v>
       </c>
-      <c r="E9" s="3">
-        <v>50</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0.42</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0.83679999999999999</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.3987</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.85540000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="3">
-        <v>23</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="5">
         <v>1.1971000000000001</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>0.3543</v>
       </c>
-      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D26" s="8"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{C74C91FC-310B-41B0-AF77-75CE81639F0D}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{78063550-A070-42A2-9978-EAFA7278F435}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{4D95AC20-094A-4630-B96D-90BA71334475}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{14694454-28DE-469C-9AD8-83C98A0AEE44}"/>
-    <hyperlink ref="C9" r:id="rId5" xr:uid="{DC2A601F-19B2-4279-B5C6-5C2B9582CDB2}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{B929C193-25B6-4F14-BAE6-B5853B3F67FC}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{E95F2D5D-5C40-41F9-98DF-1BEC8D36AA88}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{37C3ED3C-7E81-40BB-877B-B7D4A9220E33}"/>
-    <hyperlink ref="C7" r:id="rId9" xr:uid="{38A286B7-2A34-43DF-BA17-1D5DC4838BE5}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C74C91FC-310B-41B0-AF77-75CE81639F0D}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{78063550-A070-42A2-9978-EAFA7278F435}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{4D95AC20-094A-4630-B96D-90BA71334475}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{14694454-28DE-469C-9AD8-83C98A0AEE44}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{DC2A601F-19B2-4279-B5C6-5C2B9582CDB2}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{B929C193-25B6-4F14-BAE6-B5853B3F67FC}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{E95F2D5D-5C40-41F9-98DF-1BEC8D36AA88}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{37C3ED3C-7E81-40BB-877B-B7D4A9220E33}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{38A286B7-2A34-43DF-BA17-1D5DC4838BE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
@@ -1394,12 +1457,391 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF41EBD-0CE0-4A16-BBB3-D7F28220889E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="110" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7">
+        <v>30</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.19089999999999999</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.6881999999999999</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.66149999999999998</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5">
+        <v>30</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.13539999999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.95479999999999998</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2.6053000000000002</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.61809999999999998</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>30</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.24229999999999999</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.95509999999999995</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.68920000000000003</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5">
+        <v>50</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.92779999999999996</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>50</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.2344</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.91790000000000005</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.37940000000000002</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.84489999999999998</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>50</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.2344</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.91790000000000005</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.37940000000000002</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.84489999999999998</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3">
+        <v>50</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.96940000000000004</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.35070000000000001</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.87160000000000004</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.3987</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.85540000000000005</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.36030000000000001</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.86529999999999996</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.30609999999999998</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.87480000000000002</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{4A0F9884-AD69-4B33-AEAA-A4B9472718B2}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{3C72708C-361E-420B-9310-B596D5BD14CF}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{B59D1640-6DFD-4618-8E9B-B5B85A9BB308}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{9E3FFF42-C535-479B-BABC-98B60CBA024A}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{F86F6F89-F085-4FA1-A31C-DBD26972565B}"/>
+    <hyperlink ref="I5" r:id="rId6" xr:uid="{A7DD72BB-69CC-48ED-B1E4-13AA3735C71F}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{7FB6EAAD-CEAF-480C-BF93-728226BFE0F8}"/>
+    <hyperlink ref="I10" r:id="rId8" xr:uid="{788C7286-1EFA-4EEE-BA8F-380B814A0EB9}"/>
+    <hyperlink ref="I7" r:id="rId9" xr:uid="{5F48B62D-84DA-47A1-A5BE-2E8834ED8856}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>